<commit_message>
New logic of operation break at color validation of delay check is added. specially for the weekend breaks
</commit_message>
<xml_diff>
--- a/input_data/NewData_121822.xlsx
+++ b/input_data/NewData_121822.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11496"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11496" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MachineAvailability" sheetId="6" r:id="rId1"/>
@@ -488,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A130" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
@@ -3379,7 +3379,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D152" s="5">
-        <f t="shared" ref="D123:D186" si="6">B152+1</f>
+        <f t="shared" ref="D152:D186" si="6">B152+1</f>
         <v>44593</v>
       </c>
       <c r="E152" s="3">
@@ -8008,8 +8008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H874"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:G4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -8070,7 +8070,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="18">
-        <v>4</v>
+        <v>900</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1">

</xml_diff>